<commit_message>
updates to metadata relfecting NAs in cover and substrate and keywords
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_ongoing_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_ongoing_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/VA/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4C5C8F-F1A3-5B4F-99A2-52AFC3B833DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E592004-94F0-E343-B013-5FB2331FB0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="920" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>name</t>
   </si>
@@ -220,9 +220,6 @@
     <t>Feather ongoing snorkel survey</t>
   </si>
   <si>
-    <t>HR&amp;L</t>
-  </si>
-  <si>
     <t>DWR</t>
   </si>
   <si>
@@ -230,6 +227,24 @@
   </si>
   <si>
     <t>Healthy Rivers and Landscapes</t>
+  </si>
+  <si>
+    <t>o. mykiss</t>
+  </si>
+  <si>
+    <t>chinook salmon</t>
+  </si>
+  <si>
+    <t>pikeminnow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sacramento sucker </t>
+  </si>
+  <si>
+    <t>cypriniform</t>
+  </si>
+  <si>
+    <t>tule perch</t>
   </si>
 </sst>
 </file>
@@ -769,10 +784,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -790,7 +805,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -820,12 +835,32 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -962,10 +997,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
         <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes filenames and updates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_ongoing_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_ongoing_snorkel_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/VA/edi-feather-snorkel/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E592004-94F0-E343-B013-5FB2331FB0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D98BEA-1C6B-0546-B2D8-81554DA41C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="920" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="920" windowWidth="25820" windowHeight="15500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>name</t>
   </si>
@@ -220,31 +220,34 @@
     <t>Feather ongoing snorkel survey</t>
   </si>
   <si>
+    <t>Healthy Rivers and Landscapes</t>
+  </si>
+  <si>
+    <t>o. mykiss</t>
+  </si>
+  <si>
+    <t>chinook salmon</t>
+  </si>
+  <si>
+    <t>pikeminnow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sacramento sucker </t>
+  </si>
+  <si>
+    <t>cypriniform</t>
+  </si>
+  <si>
+    <t>tule perch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California Department of Water Resources </t>
+  </si>
+  <si>
     <t>DWR</t>
   </si>
   <si>
-    <t xml:space="preserve">Department of Water Resources </t>
-  </si>
-  <si>
-    <t>Healthy Rivers and Landscapes</t>
-  </si>
-  <si>
-    <t>o. mykiss</t>
-  </si>
-  <si>
-    <t>chinook salmon</t>
-  </si>
-  <si>
-    <t>pikeminnow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sacramento sucker </t>
-  </si>
-  <si>
-    <t>cypriniform</t>
-  </si>
-  <si>
-    <t>tule perch</t>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -786,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -805,7 +808,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -835,32 +838,32 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -969,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -997,10 +1000,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" t="s">
-        <v>64</v>
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to abstract, methods to md
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_ongoing_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_ongoing_snorkel_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D98BEA-1C6B-0546-B2D8-81554DA41C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EE6362-8FF3-624F-A259-C547395928AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="920" windowWidth="25820" windowHeight="15500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61540" yWindow="3660" windowWidth="28780" windowHeight="23020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -202,9 +202,6 @@
     <t>annually</t>
   </si>
   <si>
-    <t>Distribution and habitat use of juvenile Feather River salmonids</t>
-  </si>
-  <si>
     <t>habitat</t>
   </si>
   <si>
@@ -248,6 +245,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Distribution and habitat use of juvenile Feather River salmonids: 25 years and ongoing of snorkel surveys</t>
   </si>
 </sst>
 </file>
@@ -626,7 +626,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -687,7 +687,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -773,10 +773,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -808,12 +808,12 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -833,37 +833,37 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -972,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1000,16 +1000,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>71</v>
       </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating some of the metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_ongoing_snorkel_metadata.xlsx
+++ b/data-raw/metadata/feather_ongoing_snorkel_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/VA/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5940DD6-0767-7540-A60B-98DC568DEB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC225D7-22EE-C649-99AC-248CF139B55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10440" yWindow="500" windowWidth="18360" windowHeight="15760" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
   <si>
     <t>name</t>
   </si>
@@ -248,6 +248,33 @@
   </si>
   <si>
     <t>Distribution and habitat use of juvenile Feather River salmonids: 25 years and ongoing of snorkel surveys</t>
+  </si>
+  <si>
+    <t>steelhead trout </t>
+  </si>
+  <si>
+    <t>Animalia</t>
+  </si>
+  <si>
+    <t>Chordata</t>
+  </si>
+  <si>
+    <t>Actinopterygii</t>
+  </si>
+  <si>
+    <t>Salmoniformes</t>
+  </si>
+  <si>
+    <t>Salmonidae</t>
+  </si>
+  <si>
+    <t>Oncorhynchus</t>
+  </si>
+  <si>
+    <t>mykiss</t>
+  </si>
+  <si>
+    <t>Craniata</t>
   </si>
 </sst>
 </file>
@@ -642,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -684,10 +711,58 @@
       <c r="A2" t="s">
         <v>52</v>
       </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -972,7 +1047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>